<commit_message>
end points added in enum,to avoid hard coding
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\UserAPIAutomation\UserApiRESTAssured\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF1A91C-4094-4B68-9FA0-292BF6F0F421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36CD45D-4F24-440D-84C5-6EB9272E333C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-760" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Scenario</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>234567765</t>
+  </si>
+  <si>
+    <t>200</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D707F8-301A-46D5-9FD2-5F3752A18AA4}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,12 +699,48 @@
         <v>46</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{D7DD8443-134F-4AA3-8E57-079B9543B2B4}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{2C5B6DEA-CE67-4255-BCCD-0CB7448A6EA9}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{2E44D5DE-B10A-4B0B-B289-604427C13627}"/>
     <hyperlink ref="D7" r:id="rId4" xr:uid="{E1285561-FA2E-46BE-B89E-80D8EF54DFBF}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{7A89A656-3DFC-4546-AD3B-F9695E8403AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
To make scalable removed row number
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinza\UserAPIAutomation\UserApiRESTAssured\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36CD45D-4F24-440D-84C5-6EB9272E333C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04E7557-7D16-4CAD-9700-129FE09C0802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-760" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>Scenario</t>
   </si>
@@ -57,9 +57,6 @@
     <t>ExpectedStatus</t>
   </si>
   <si>
-    <t>ExpectedMessage</t>
-  </si>
-  <si>
     <t>plotNumber</t>
   </si>
   <si>
@@ -105,45 +102,12 @@
     <t>User created successfully</t>
   </si>
   <si>
-    <t>ValidUser</t>
-  </si>
-  <si>
     <t>123455</t>
   </si>
   <si>
     <t>123454</t>
   </si>
   <si>
-    <t>1631794236</t>
-  </si>
-  <si>
-    <t>2345492347</t>
-  </si>
-  <si>
-    <t>6619797219</t>
-  </si>
-  <si>
-    <t>uort796@gmail.com</t>
-  </si>
-  <si>
-    <t>orer79521@gmail.com</t>
-  </si>
-  <si>
-    <t>wer2963@gmail.com</t>
-  </si>
-  <si>
-    <t>wer234gmail.com</t>
-  </si>
-  <si>
-    <t>2345678987</t>
-  </si>
-  <si>
-    <t>1234567823</t>
-  </si>
-  <si>
-    <t>InvalidUser</t>
-  </si>
-  <si>
     <t>topu</t>
   </si>
   <si>
@@ -162,20 +126,89 @@
     <t>asdf</t>
   </si>
   <si>
-    <t>wert34@gmail.com</t>
-  </si>
-  <si>
-    <t>234567765</t>
-  </si>
-  <si>
     <t>200</t>
+  </si>
+  <si>
+    <t>RequestType</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>Bad request</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Updated Successfully</t>
+  </si>
+  <si>
+    <t>wer23994gmail.com</t>
+  </si>
+  <si>
+    <t>wert3994@gmail.com</t>
+  </si>
+  <si>
+    <t>orer79999521@gmail.com</t>
+  </si>
+  <si>
+    <t>orer79995881@gmail.com</t>
+  </si>
+  <si>
+    <t>1234126794</t>
+  </si>
+  <si>
+    <t>1234126795</t>
+  </si>
+  <si>
+    <t>Valid Data</t>
+  </si>
+  <si>
+    <t>Invalid Data</t>
+  </si>
+  <si>
+    <t>ExpectedStatusLine</t>
+  </si>
+  <si>
+    <t>ras456@gmail.com</t>
+  </si>
+  <si>
+    <t>was695@gmail.com</t>
+  </si>
+  <si>
+    <t>uort123@gmail.com</t>
+  </si>
+  <si>
+    <t>1234127592</t>
+  </si>
+  <si>
+    <t>1234124593</t>
+  </si>
+  <si>
+    <t>5534129789</t>
+  </si>
+  <si>
+    <t>1866453490</t>
+  </si>
+  <si>
+    <t>1239409878</t>
+  </si>
+  <si>
+    <t>ploy-76</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +220,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -499,22 +538,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D707F8-301A-46D5-9FD2-5F3752A18AA4}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +574,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -546,201 +589,290 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
+      <c r="M1" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="K4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="M8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="1">
-        <v>201</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="1">
-        <v>201</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="1">
-        <v>201</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="K9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{D7DD8443-134F-4AA3-8E57-079B9543B2B4}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{2C5B6DEA-CE67-4255-BCCD-0CB7448A6EA9}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{2E44D5DE-B10A-4B0B-B289-604427C13627}"/>
     <hyperlink ref="D7" r:id="rId4" xr:uid="{E1285561-FA2E-46BE-B89E-80D8EF54DFBF}"/>
     <hyperlink ref="D8" r:id="rId5" xr:uid="{7A89A656-3DFC-4546-AD3B-F9695E8403AD}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{FB4DCA33-4BEB-4DD5-82AF-7978FC3CADAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>